<commit_message>
click on selected to deselect, fixed some job font-colors and descriptions, selected div goes to negative z which brings it to the top and not subject to parallax
</commit_message>
<xml_diff>
--- a/version-0.5/static_content/jobs/jobs.xlsx
+++ b/version-0.5/static_content/jobs/jobs.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/version-0.5/static_content/jobs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C25EF1-4647-5C4D-BF5F-04BBC830C9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-63880" yWindow="3060" windowWidth="28580" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="jobs" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="jobs"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -64,19 +58,28 @@
     <t>#008b8b</t>
   </si>
   <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>• Working as a consulting data engineer in the data cyber security team of the [Cigna Group](url).</t>
+  </si>
+  <si>
+    <t>Warner Brothers Interactive Entertainment</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>#0000ff</t>
+  </si>
+  <si>
     <t>white</t>
   </si>
   <si>
-    <t>• Working as a consulting data engineer in the data cyber security team of the [Cigna Group](url).</t>
-  </si>
-  <si>
-    <t>Warner Brothers Interactive Entertainment</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>#0000ff</t>
+    <t>• Worked as a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](url) Division.
+• Implemented high-volume pipeline integrations shuffling game telemetry and [user PII data](URL) between WB-distributed consumer games and [marketing service platforms](URL) via [Segment customer data platform](url) using [Kafka](url), [Redshift](url), and [Airflow](url). 
+• Employed [Python](url), [Amazon Glue](url) and [Apache Airflow](url) for external [3rd-party integrations](url) and internal [dev-ops integrations](url) with [Jenkins](url), [DataDog](url), and [ZenDesk](url) 
+• Integrated with [Google BigQuery](url) [data warehouse](url) and [AWS-managed services](url) [Airflow](url), [S3](url), [Glue](url), and [Redshift warehouse](url).</t>
   </si>
   <si>
     <t xml:space="preserve">Angel Studios </t>
@@ -88,6 +91,12 @@
     <t>#0000cd</t>
   </si>
   <si>
+    <t>• Worked as a consulting data engineer for [Angel Studios](url], a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
+• Used [Python](url), [Pandas](url]), [Numpy](url), [Keras](url), and [Jupyter](url) to build and tune [hyperparameters](url) of a [convolutional neural network](url) with [supervised learning](url) on [AWS Sagemaker](url) to classify movie frames from episodic programs stored in [S3](url). 
+• Built web client apps using [Python](url) with [Postman](url) that made [RESTful API](url) requests to pull monthly usage data from various web marketing partners like [FaceBook](url), [Google Play](url), and [Vimeo](url). 
+• Worked with [Segment customer data platform](url), [Excel](url), and [Tableau](url) to create scheduled [reports] for the company's sales and finance teams.</t>
+  </si>
+  <si>
     <t>Greenseed Tech</t>
   </si>
   <si>
@@ -95,6 +104,12 @@
   </si>
   <si>
     <t>#8a2be2</t>
+  </si>
+  <si>
+    <t>• Worked as a consulting data engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide.
+• [Containerized](url) legacy web applications using [Docker](url) and [AWS Secrets Manager](url). 
+• Documented existing data architecture as [ERDs](url) using [DBeaver Enterprise](url). 
+• Used [Selenium](url) and [Python](url) to [screem scrape](url) publicly available data from selected websites.</t>
   </si>
   <si>
     <t xml:space="preserve">Consulting Full-Stack Developer </t>
@@ -161,9 +176,6 @@
   </si>
   <si>
     <t>#ff4500</t>
-  </si>
-  <si>
-    <t>black</t>
   </si>
   <si>
     <t>• Co-founded a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
@@ -207,7 +219,7 @@
 • Designed datamodel and data entry tools for category-specific product attribution. 
 • Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
 • Instrumental in raising over $70M in venture capital. 
-• Used [Oracle IIi](url), [ATG Dyanamo](url), [Java 8](url), [Akamai](url), [WebTrends](url), [FileMakerPro](url), [ImageMagik](url), and Omnigraph](url) for data modeling and workflow designs.</t>
+• Used [Oracle IIi](url), [ATG Dyanamo](url), [Java 8](url), [Akamai](url), [WebTrends](url), [FileMakerPro](url), [ImageMagik](url), and [Omnigraph](url) for data modeling and workflow designs.</t>
   </si>
   <si>
     <t xml:space="preserve">Lead Software Developer </t>
@@ -373,6 +385,11 @@
     <t>#32cd32</t>
   </si>
   <si>
+    <t>• [Intrusic LLC](url) built real-time network monitoring systems that identified external and internal network intrusion attempts
+• As a Sierra Vista Group consulting architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
+• Used [Debian Linux](url), [C](url), and [Visio](url).</t>
+  </si>
+  <si>
     <t xml:space="preserve">Consulting Architect / Technical Lead </t>
   </si>
   <si>
@@ -405,36 +422,13 @@
 •  Used [Java](url), [ObjectDesign](url), [JavaScript ES3](url), [MySQL 4](url), and [Adobe Photoshop v5.0](url). 
 </t>
   </si>
-  <si>
-    <t>• Worked as a consulting data engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide.
-• [Containerized](url) legacy web applications using [Docker](url) and [AWS Secrets Manager](url). 
-• Documented existing data architecture as [ERDs](url) using [DBeaver Enterprise](url). 
-• Used [Selenium](url) and [Python](url) to [screem scrape](url) publicly available data from selected websites.</t>
-  </si>
-  <si>
-    <t>• Worked as a consulting data engineer for [Angel Studios](url], a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used [Python](url), [Pandas](url]), [Numpy](url), [Keras](url), and [Jupyter](url) to build and tune [hyperparameters](url) of a [convolutional neural network](url)with [supervised learning](url) on [AWS Sagemaker](url) to classify movie frames from episodic programs stored in [S3](url). 
-• Built web client apps using [Python](url) with [Postman](url) that made [RESTful API](url) requests to pull monthly usage data from various web marketing partners like [FaceBook](url), [Google Play](url), and [Vimeo](url). 
-• Worked with [Segment customer data platform](url), [Excel](url), and [Tableau](url) to create scheduled [reports] for the company's sales and finance teams.</t>
-  </si>
-  <si>
-    <t>• [Intrusic LLC](url) built real-time network monitoring systems that identified external and internal network intrusion attempts
-• As a Sierra Vista Group consulting architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
-• Used [Debian Linux](url), [C](url), and [Visio](url).</t>
-  </si>
-  <si>
-    <t>• Worked as a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](url) Division.
-• Implemented high-volume pipeline integrations shuffling game telemetry and [user PII data](URL) between WB-distributed consumer games and [marketing service platforms](URL) via [Segment customer data platform](url) using [Kafka](url), [Redshift](url), and [Airflow](url). 
-• Employed [Python](url), [Amazon Glue](url) and [Apache Airflow](url) for external [3rd-party integrations](url) and internal [dev-ops integrations](url) with [Jenkins](url), [DataDog](url), and (ZenDesk](url) 
-• Integrated with [Google BigQuery](url) [data warehouse](url) and [AWS-managed services](url) [Airflow](url), [S3](url), [Glue](url), and [Redshift warehouse](url).</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -453,7 +447,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -467,22 +461,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008B8B"/>
+        <fgColor rgb="FF008b8b"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
+        <fgColor rgb="FF0000ff"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000CD"/>
+        <fgColor rgb="FF0000cd"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8A2BE2"/>
+        <fgColor rgb="FF8a2be2"/>
       </patternFill>
     </fill>
     <fill>
@@ -497,17 +491,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDC143C"/>
+        <fgColor rgb="FFdc143c"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF4500"/>
+        <fgColor rgb="FFff4500"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
+        <fgColor rgb="FFffa500"/>
       </patternFill>
     </fill>
     <fill>
@@ -517,32 +511,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD700"/>
+        <fgColor rgb="FFffd700"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFffff00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
+        <fgColor rgb="FF00ff00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF32CD32"/>
+        <fgColor rgb="FF32cd32"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6B8E23"/>
+        <fgColor rgb="FF6b8e23"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF228B22"/>
+        <fgColor rgb="FF228b22"/>
       </patternFill>
     </fill>
   </fills>
@@ -581,104 +575,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -689,10 +682,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -730,71 +723,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -822,7 +815,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -845,11 +838,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -858,13 +851,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -874,7 +867,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -883,7 +876,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -892,7 +885,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -900,10 +893,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -968,27 +961,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="96" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="26" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="26" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="28" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="29" width="96.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="129.75">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1074,18 +1069,18 @@
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="157.5">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="6">
         <v>44501</v>
@@ -1097,25 +1092,25 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="88.5">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6">
         <v>44136</v>
@@ -1127,25 +1122,25 @@
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="60.75">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6">
         <v>43770</v>
@@ -1157,25 +1152,25 @@
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="168">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6">
         <v>42795</v>
@@ -1187,25 +1182,25 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="75.75">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C8" s="6">
         <v>42705</v>
@@ -1217,25 +1212,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="168">
       <c r="A9" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C9" s="6">
         <v>40575</v>
@@ -1247,25 +1242,25 @@
         <v>2</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="156.75">
+      <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6">
         <v>37561</v>
@@ -1277,25 +1272,25 @@
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="133.5">
+      <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="B11" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6">
         <v>35827</v>
@@ -1307,25 +1302,25 @@
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="75.75">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C12" s="6">
         <v>35217</v>
@@ -1347,15 +1342,15 @@
         <v>14</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="214.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="214.5">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C13" s="6">
         <v>33117</v>
@@ -1374,18 +1369,18 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="179.25">
       <c r="A14" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C14" s="6">
         <v>32021</v>
@@ -1397,25 +1392,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="40.5">
       <c r="A15" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C15" s="6">
         <v>32295</v>
@@ -1427,25 +1422,25 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C16" s="6">
         <v>30926</v>
@@ -1457,25 +1452,25 @@
         <v>2</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="40.5">
       <c r="A17" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C17" s="6">
         <v>30682</v>
@@ -1487,25 +1482,25 @@
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="29.25">
       <c r="A18" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C18" s="6">
         <v>30133</v>
@@ -1517,25 +1512,25 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C19" s="6">
         <v>29830</v>
@@ -1547,25 +1542,25 @@
         <v>2</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="40.5">
       <c r="A20" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C20" s="6">
         <v>29677</v>
@@ -1577,25 +1572,25 @@
         <v>1</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="41.25">
       <c r="A21" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C21" s="6">
         <v>28369</v>
@@ -1607,25 +1602,25 @@
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="109.5">
       <c r="A22" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C22" s="6">
         <v>39417</v>
@@ -1637,25 +1632,25 @@
         <v>2</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="75.75">
       <c r="A23" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C23" s="6">
         <v>38749</v>
@@ -1667,25 +1662,25 @@
         <v>2</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="63.75">
       <c r="A24" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C24" s="6">
         <v>38384</v>
@@ -1697,25 +1692,25 @@
         <v>2</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="63.75">
       <c r="A25" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C25" s="6">
         <v>38018</v>
@@ -1727,25 +1722,25 @@
         <v>2</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J25" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="87.75">
+      <c r="A26" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="B26" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C26" s="6">
         <v>37681</v>
@@ -1757,17 +1752,17 @@
         <v>2</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H26" s="25"/>
       <c r="I26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>